<commit_message>
start of the day
</commit_message>
<xml_diff>
--- a/Stella weekly hours.xlsx
+++ b/Stella weekly hours.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27531"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27628"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://universitetetitromso-my.sharepoint.com/personal/stpis0397_uit_no/Documents/LESS-Project-with-RAs-2/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="176" documentId="11_F25DC773A252ABDACC104886F99C55E85BDE58ED" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{AC287E0B-A3B4-4B62-AACB-742471FB9B47}"/>
+  <xr:revisionPtr revIDLastSave="179" documentId="11_F25DC773A252ABDACC104886F99C55E85BDE58ED" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8759D62D-3439-4D5F-A3D7-B52B142D1404}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -89,10 +89,10 @@
     <t>preprocessing session 4</t>
   </si>
   <si>
-    <t>preprocessing session 4 and trial by trial pipeline session 2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">6, 45 + 5, 15 </t>
+    <t xml:space="preserve">18, 45 </t>
+  </si>
+  <si>
+    <t>preprocessing session 4 and trial by trial pipeline session 2, 3, 4</t>
   </si>
 </sst>
 </file>
@@ -494,7 +494,7 @@
   <dimension ref="A1:D28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -664,10 +664,10 @@
         <v>45488</v>
       </c>
       <c r="B14" t="s">
+        <v>15</v>
+      </c>
+      <c r="C14" t="s">
         <v>16</v>
-      </c>
-      <c r="C14" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">

</xml_diff>